<commit_message>
Testing and bug fixed
</commit_message>
<xml_diff>
--- a/double_dabble_combinational/performance_test.xlsx
+++ b/double_dabble_combinational/performance_test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Reg</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>LUT</t>
-  </si>
-  <si>
-    <t>Freq</t>
   </si>
   <si>
     <t>MaxValue</t>
@@ -83,11 +80,29 @@
   <si>
     <t>9</t>
   </si>
+  <si>
+    <t>Sequential implementation</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Freq [MHz]</t>
+  </si>
+  <si>
+    <t>Time [ns]</t>
+  </si>
+  <si>
+    <t>Lepsze Freq</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -117,10 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -415,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="8" ySplit="2" topLeftCell="I9" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -431,37 +447,47 @@
     <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="15.375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="4.875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="4.25" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5" hidden="1" customWidth="1"/>
+    <col min="15" max="18" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:22">
       <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -473,10 +499,37 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>1</v>
       </c>
@@ -519,8 +572,35 @@
       <c r="L3">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <f>1/L3*1000</f>
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <f>C3*4</f>
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>19</v>
+      </c>
+      <c r="Q3">
+        <v>12</v>
+      </c>
+      <c r="R3">
+        <v>21</v>
+      </c>
+      <c r="S3">
+        <v>251</v>
+      </c>
+      <c r="V3" t="str">
+        <f>IF(L3&gt;S3,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>2</v>
       </c>
@@ -563,8 +643,35 @@
       <c r="L4">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N34" si="5">1/L4*1000</f>
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O34" si="6">C4*4</f>
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>21</v>
+      </c>
+      <c r="Q4">
+        <v>13</v>
+      </c>
+      <c r="R4">
+        <v>22</v>
+      </c>
+      <c r="S4">
+        <v>301</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" ref="V4:V34" si="7">IF(L4&gt;S4,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>3</v>
       </c>
@@ -607,8 +714,35 @@
       <c r="L5">
         <v>500</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>21</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <v>16</v>
+      </c>
+      <c r="S5">
+        <v>321</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="7"/>
+        <v>Comb</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>4</v>
       </c>
@@ -651,8 +785,35 @@
       <c r="L6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>37</v>
+      </c>
+      <c r="Q6">
+        <v>21</v>
+      </c>
+      <c r="R6">
+        <v>32</v>
+      </c>
+      <c r="S6">
+        <v>266</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="7"/>
+        <v>Comb</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>5</v>
       </c>
@@ -695,8 +856,35 @@
       <c r="L7">
         <v>483</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="5"/>
+        <v>2.0703933747412009</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P7">
+        <v>39</v>
+      </c>
+      <c r="Q7">
+        <v>22</v>
+      </c>
+      <c r="R7">
+        <v>32</v>
+      </c>
+      <c r="S7">
+        <v>262</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="7"/>
+        <v>Comb</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>6</v>
       </c>
@@ -739,8 +927,38 @@
       <c r="L8">
         <v>174</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="5"/>
+        <v>5.7471264367816088</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P8">
+        <v>42</v>
+      </c>
+      <c r="Q8">
+        <v>25</v>
+      </c>
+      <c r="R8">
+        <v>36</v>
+      </c>
+      <c r="S8">
+        <v>271</v>
+      </c>
+      <c r="T8">
+        <v>13</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>7</v>
       </c>
@@ -783,8 +1001,38 @@
       <c r="L9">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="5"/>
+        <v>7.9365079365079358</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="P9">
+        <v>44</v>
+      </c>
+      <c r="Q9">
+        <v>24</v>
+      </c>
+      <c r="R9">
+        <v>37</v>
+      </c>
+      <c r="S9">
+        <v>221</v>
+      </c>
+      <c r="T9">
+        <v>15</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>8</v>
       </c>
@@ -827,8 +1075,38 @@
       <c r="L10">
         <v>149</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="5"/>
+        <v>6.7114093959731544</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="P10">
+        <v>58</v>
+      </c>
+      <c r="Q10">
+        <v>32</v>
+      </c>
+      <c r="R10">
+        <v>44</v>
+      </c>
+      <c r="S10">
+        <v>170</v>
+      </c>
+      <c r="T10">
+        <v>17</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>9</v>
       </c>
@@ -871,8 +1149,35 @@
       <c r="L11">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="5"/>
+        <v>11.494252873563218</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="P11">
+        <v>60</v>
+      </c>
+      <c r="Q11">
+        <v>32</v>
+      </c>
+      <c r="R11">
+        <v>42</v>
+      </c>
+      <c r="S11">
+        <v>233</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>10</v>
       </c>
@@ -915,8 +1220,38 @@
       <c r="L12">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="5"/>
+        <v>16.129032258064516</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="P12">
+        <v>75</v>
+      </c>
+      <c r="Q12">
+        <v>41</v>
+      </c>
+      <c r="R12">
+        <v>55</v>
+      </c>
+      <c r="S12">
+        <v>233</v>
+      </c>
+      <c r="T12">
+        <v>21</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>11</v>
       </c>
@@ -959,8 +1294,38 @@
       <c r="L13">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="5"/>
+        <v>16.129032258064516</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="P13">
+        <v>77</v>
+      </c>
+      <c r="Q13">
+        <v>42</v>
+      </c>
+      <c r="R13">
+        <v>56</v>
+      </c>
+      <c r="S13">
+        <v>207</v>
+      </c>
+      <c r="T13">
+        <v>23</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1003,8 +1368,38 @@
       <c r="L14">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="5"/>
+        <v>19.230769230769234</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="P14">
+        <v>79</v>
+      </c>
+      <c r="Q14">
+        <v>43</v>
+      </c>
+      <c r="R14">
+        <v>57</v>
+      </c>
+      <c r="S14">
+        <v>194</v>
+      </c>
+      <c r="T14">
+        <v>25</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1047,8 +1442,38 @@
       <c r="L15">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="5"/>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="P15">
+        <v>81</v>
+      </c>
+      <c r="Q15">
+        <v>42</v>
+      </c>
+      <c r="R15">
+        <v>59</v>
+      </c>
+      <c r="S15">
+        <v>206</v>
+      </c>
+      <c r="T15">
+        <v>27</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1091,8 +1516,38 @@
       <c r="L16">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="5"/>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="P16">
+        <v>95</v>
+      </c>
+      <c r="Q16">
+        <v>51</v>
+      </c>
+      <c r="R16">
+        <v>67</v>
+      </c>
+      <c r="S16">
+        <v>216</v>
+      </c>
+      <c r="T16">
+        <v>29</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1135,8 +1590,38 @@
       <c r="L17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="5"/>
+        <v>31.25</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="P17">
+        <v>97</v>
+      </c>
+      <c r="Q17">
+        <v>51</v>
+      </c>
+      <c r="R17">
+        <v>68</v>
+      </c>
+      <c r="S17">
+        <v>204</v>
+      </c>
+      <c r="T17">
+        <v>31</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1179,8 +1664,38 @@
       <c r="L18">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="5"/>
+        <v>32.258064516129032</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="P18">
+        <v>99</v>
+      </c>
+      <c r="Q18">
+        <v>52</v>
+      </c>
+      <c r="R18">
+        <v>68</v>
+      </c>
+      <c r="S18">
+        <v>208</v>
+      </c>
+      <c r="T18">
+        <v>33</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1223,8 +1738,35 @@
       <c r="L19">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="5"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="P19">
+        <v>113</v>
+      </c>
+      <c r="Q19">
+        <v>58</v>
+      </c>
+      <c r="R19">
+        <v>74</v>
+      </c>
+      <c r="S19">
+        <v>203</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1267,8 +1809,38 @@
       <c r="L20">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="5"/>
+        <v>38.461538461538467</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="P20">
+        <v>116</v>
+      </c>
+      <c r="Q20">
+        <v>62</v>
+      </c>
+      <c r="R20">
+        <v>80</v>
+      </c>
+      <c r="S20">
+        <v>154</v>
+      </c>
+      <c r="T20">
+        <v>37</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1311,8 +1883,38 @@
       <c r="L21">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="P21">
+        <v>118</v>
+      </c>
+      <c r="Q21">
+        <v>62</v>
+      </c>
+      <c r="R21">
+        <v>81</v>
+      </c>
+      <c r="S21">
+        <v>161</v>
+      </c>
+      <c r="T21">
+        <v>39</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1355,8 +1957,35 @@
       <c r="L22">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="5"/>
+        <v>43.478260869565219</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="P22">
+        <v>132</v>
+      </c>
+      <c r="Q22">
+        <v>69</v>
+      </c>
+      <c r="R22">
+        <v>89</v>
+      </c>
+      <c r="S22">
+        <v>175</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1399,8 +2028,35 @@
       <c r="L23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="5"/>
+        <v>45.454545454545453</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="P23">
+        <v>134</v>
+      </c>
+      <c r="Q23">
+        <v>70</v>
+      </c>
+      <c r="R23">
+        <v>90</v>
+      </c>
+      <c r="S23">
+        <v>147</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1443,8 +2099,35 @@
       <c r="L24">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="5"/>
+        <v>47.619047619047613</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="P24">
+        <v>136</v>
+      </c>
+      <c r="Q24">
+        <v>73</v>
+      </c>
+      <c r="R24">
+        <v>91</v>
+      </c>
+      <c r="S24">
+        <v>161</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1487,8 +2170,35 @@
       <c r="L25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="P25">
+        <v>138</v>
+      </c>
+      <c r="Q25">
+        <v>72</v>
+      </c>
+      <c r="R25">
+        <v>92</v>
+      </c>
+      <c r="S25">
+        <v>192</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1531,8 +2241,35 @@
       <c r="L26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="P26">
+        <v>152</v>
+      </c>
+      <c r="Q26">
+        <v>80</v>
+      </c>
+      <c r="R26">
+        <v>100</v>
+      </c>
+      <c r="S26">
+        <v>165</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1575,8 +2312,35 @@
       <c r="L27">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3">
+        <f t="shared" si="5"/>
+        <v>52.631578947368418</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="P27">
+        <v>154</v>
+      </c>
+      <c r="Q27">
+        <v>79</v>
+      </c>
+      <c r="R27">
+        <v>101</v>
+      </c>
+      <c r="S27">
+        <v>158</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1619,8 +2383,35 @@
       <c r="L28">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" si="5"/>
+        <v>52.631578947368418</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="P28">
+        <v>156</v>
+      </c>
+      <c r="Q28">
+        <v>81</v>
+      </c>
+      <c r="R28">
+        <v>102</v>
+      </c>
+      <c r="S28">
+        <v>169</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1663,8 +2454,35 @@
       <c r="L29">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" si="5"/>
+        <v>55.55555555555555</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="P29">
+        <v>170</v>
+      </c>
+      <c r="Q29">
+        <v>88</v>
+      </c>
+      <c r="R29">
+        <v>110</v>
+      </c>
+      <c r="S29">
+        <v>170</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1707,8 +2525,35 @@
       <c r="L30">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <f t="shared" si="5"/>
+        <v>55.55555555555555</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="P30">
+        <v>172</v>
+      </c>
+      <c r="Q30">
+        <v>89</v>
+      </c>
+      <c r="R30">
+        <v>111</v>
+      </c>
+      <c r="S30">
+        <v>171</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1751,8 +2596,35 @@
       <c r="L31">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" si="5"/>
+        <v>58.823529411764703</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="P31">
+        <v>174</v>
+      </c>
+      <c r="Q31">
+        <v>89</v>
+      </c>
+      <c r="R31">
+        <v>113</v>
+      </c>
+      <c r="S31">
+        <v>176</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1795,8 +2667,35 @@
       <c r="L32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32" s="3">
+        <f t="shared" si="5"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="P32">
+        <v>188</v>
+      </c>
+      <c r="Q32">
+        <v>98</v>
+      </c>
+      <c r="R32">
+        <v>121</v>
+      </c>
+      <c r="S32">
+        <v>144</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1839,8 +2738,35 @@
       <c r="L33">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33" s="3">
+        <f t="shared" si="5"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="P33">
+        <v>190</v>
+      </c>
+      <c r="Q33">
+        <v>97</v>
+      </c>
+      <c r="R33">
+        <v>122</v>
+      </c>
+      <c r="S33">
+        <v>170</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1882,6 +2808,33 @@
       </c>
       <c r="L34">
         <v>15</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="5"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="P34">
+        <v>192</v>
+      </c>
+      <c r="Q34">
+        <v>99</v>
+      </c>
+      <c r="R34">
+        <v>122</v>
+      </c>
+      <c r="S34">
+        <v>173</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="7"/>
+        <v>Seq</v>
       </c>
     </row>
   </sheetData>
@@ -1902,7 +2855,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1910,7 +2863,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1918,7 +2871,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1926,7 +2879,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1934,7 +2887,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1942,7 +2895,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1950,7 +2903,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1958,7 +2911,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1966,7 +2919,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>4</v>

</xml_diff>

<commit_message>
Comparison between sequential and combinational implementation
</commit_message>
<xml_diff>
--- a/double_dabble_combinational/performance_test.xlsx
+++ b/double_dabble_combinational/performance_test.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27960" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27960" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Wykresy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Reg</t>
   </si>
@@ -104,6 +104,9 @@
   <si>
     <t>Mniej LUT</t>
   </si>
+  <si>
+    <t>Porównanie</t>
+  </si>
 </sst>
 </file>
 
@@ -153,6 +156,843 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Combinational</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$A$3:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$L$3:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$3:$S$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="1">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>159</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="40817408"/>
+        <c:axId val="40818944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="40817408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40818944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="40818944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40817408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Combinational</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$A$3:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$J$3:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$Q$3:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="62596992"/>
+        <c:axId val="62598528"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="62596992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62598528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="62598528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="62596992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,13 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -456,24 +1293,27 @@
     <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="15.375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="4.875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="4.25" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="4.875" customWidth="1"/>
+    <col min="11" max="11" width="4.25" customWidth="1"/>
+    <col min="12" max="12" width="9.875" customWidth="1"/>
+    <col min="13" max="13" width="6.5" customWidth="1"/>
+    <col min="14" max="14" width="8.5" customWidth="1"/>
     <col min="15" max="18" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="I1" t="s">
+    <row r="1" spans="1:25">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
       </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -535,19 +1375,22 @@
         <v>22</v>
       </c>
       <c r="U2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>27</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>28</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -601,12 +1444,12 @@
         <f>C3*4</f>
         <v>4</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <f>IF(L3&gt;S3,"Comb","Seq")</f>
         <v>Comb</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -667,20 +1510,36 @@
         <v>12</v>
       </c>
       <c r="R4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S4">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="T4">
         <v>5</v>
       </c>
+      <c r="U4" s="3">
+        <f>T4/S4*1000</f>
+        <v>17.730496453900709</v>
+      </c>
+      <c r="V4" t="str">
+        <f>IF(I4&lt;P4,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
+      <c r="W4" t="str">
+        <f>IF(J4&lt;Q4,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
       <c r="X4" t="str">
-        <f t="shared" ref="X4:X34" si="7">IF(L4&gt;S4,"Comb","Seq")</f>
+        <f>IF(K4&lt;R4,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" ref="Y4:Y34" si="7">IF(L4&gt;S4,"Comb","Seq")</f>
         <v>Comb</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -735,26 +1594,42 @@
         <v>4</v>
       </c>
       <c r="P5">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="Q5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R5">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="S5">
-        <v>321</v>
+        <v>281</v>
       </c>
       <c r="T5">
         <v>7</v>
       </c>
+      <c r="U5" s="3">
+        <f t="shared" ref="U5:U34" si="8">T5/S5*1000</f>
+        <v>24.911032028469752</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" ref="V5:V34" si="9">IF(I5&lt;P5,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" ref="W5:W34" si="10">IF(J5&lt;Q5,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
       <c r="X5" t="str">
+        <f t="shared" ref="X5:X34" si="11">IF(K5&lt;R5,"Comb","Seq")</f>
+        <v>Comb</v>
+      </c>
+      <c r="Y5" t="str">
         <f t="shared" si="7"/>
         <v>Comb</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -818,17 +1693,33 @@
         <v>32</v>
       </c>
       <c r="S6">
-        <v>266</v>
+        <v>208</v>
       </c>
       <c r="T6">
         <v>9</v>
       </c>
+      <c r="U6" s="3">
+        <f t="shared" si="8"/>
+        <v>43.269230769230766</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X6" t="str">
+        <f t="shared" si="11"/>
+        <v>Comb</v>
+      </c>
+      <c r="Y6" t="str">
         <f t="shared" si="7"/>
         <v>Comb</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -883,26 +1774,42 @@
         <v>8</v>
       </c>
       <c r="P7">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q7">
         <v>22</v>
       </c>
       <c r="R7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="S7">
-        <v>262</v>
+        <v>223</v>
       </c>
       <c r="T7">
         <v>11</v>
       </c>
+      <c r="U7" s="3">
+        <f t="shared" si="8"/>
+        <v>49.327354260089685</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X7" t="str">
+        <f t="shared" si="11"/>
+        <v>Comb</v>
+      </c>
+      <c r="Y7" t="str">
         <f t="shared" si="7"/>
         <v>Comb</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -963,20 +1870,36 @@
         <v>25</v>
       </c>
       <c r="R8">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S8">
-        <v>271</v>
+        <v>208</v>
       </c>
       <c r="T8">
         <v>13</v>
       </c>
+      <c r="U8" s="3">
+        <f t="shared" si="8"/>
+        <v>62.5</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X8" t="str">
+        <f t="shared" si="11"/>
+        <v>Comb</v>
+      </c>
+      <c r="Y8" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1031,26 +1954,42 @@
         <v>12</v>
       </c>
       <c r="P9">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="Q9">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="R9">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="S9">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="T9">
         <v>15</v>
       </c>
+      <c r="U9" s="3">
+        <f t="shared" si="8"/>
+        <v>66.964285714285708</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X9" t="str">
+        <f t="shared" si="11"/>
+        <v>Comb</v>
+      </c>
+      <c r="Y9" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1114,17 +2053,33 @@
         <v>44</v>
       </c>
       <c r="S10">
-        <v>170</v>
+        <v>213</v>
       </c>
       <c r="T10">
         <v>17</v>
       </c>
+      <c r="U10" s="3">
+        <f t="shared" si="8"/>
+        <v>79.812206572769952</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X10" t="str">
+        <f t="shared" si="11"/>
+        <v>Comb</v>
+      </c>
+      <c r="Y10" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1179,26 +2134,42 @@
         <v>12</v>
       </c>
       <c r="P11">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R11">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="S11">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="T11">
         <v>19</v>
       </c>
+      <c r="U11" s="3">
+        <f t="shared" si="8"/>
+        <v>84.821428571428569</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X11" t="str">
+        <f t="shared" si="11"/>
+        <v>Comb</v>
+      </c>
+      <c r="Y11" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1259,20 +2230,36 @@
         <v>41</v>
       </c>
       <c r="R12">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S12">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="T12">
         <v>21</v>
       </c>
+      <c r="U12" s="3">
+        <f t="shared" si="8"/>
+        <v>95.454545454545453</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X12" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y12" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1333,20 +2320,36 @@
         <v>42</v>
       </c>
       <c r="R13">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S13">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="T13">
         <v>23</v>
       </c>
+      <c r="U13" s="3">
+        <f t="shared" si="8"/>
+        <v>105.02283105022831</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" si="10"/>
+        <v>Comb</v>
+      </c>
       <c r="X13" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y13" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1407,20 +2410,36 @@
         <v>43</v>
       </c>
       <c r="R14">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S14">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="T14">
         <v>25</v>
       </c>
+      <c r="U14" s="3">
+        <f t="shared" si="8"/>
+        <v>116.27906976744185</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X14" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y14" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1481,20 +2500,36 @@
         <v>42</v>
       </c>
       <c r="R15">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S15">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="T15">
         <v>27</v>
       </c>
+      <c r="U15" s="3">
+        <f t="shared" si="8"/>
+        <v>116.88311688311688</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X15" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y15" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1555,20 +2590,36 @@
         <v>51</v>
       </c>
       <c r="R16">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S16">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="T16">
         <v>29</v>
       </c>
+      <c r="U16" s="3">
+        <f t="shared" si="8"/>
+        <v>148.71794871794873</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X16" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y16" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1629,20 +2680,36 @@
         <v>51</v>
       </c>
       <c r="R17">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S17">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="T17">
         <v>31</v>
       </c>
+      <c r="U17" s="3">
+        <f t="shared" si="8"/>
+        <v>147.61904761904762</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X17" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y17" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1703,20 +2770,36 @@
         <v>52</v>
       </c>
       <c r="R18">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S18">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="T18">
         <v>33</v>
       </c>
+      <c r="U18" s="3">
+        <f t="shared" si="8"/>
+        <v>144.73684210526315</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X18" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y18" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1771,26 +2854,42 @@
         <v>24</v>
       </c>
       <c r="P19">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q19">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R19">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S19">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="T19">
         <v>35</v>
       </c>
+      <c r="U19" s="3">
+        <f t="shared" si="8"/>
+        <v>204.67836257309941</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X19" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y19" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1851,20 +2950,36 @@
         <v>62</v>
       </c>
       <c r="R20">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S20">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="T20">
         <v>37</v>
       </c>
+      <c r="U20" s="3">
+        <f t="shared" si="8"/>
+        <v>229.81366459627327</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X20" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y20" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1925,20 +3040,36 @@
         <v>62</v>
       </c>
       <c r="R21">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S21">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="T21">
         <v>39</v>
       </c>
+      <c r="U21" s="3">
+        <f t="shared" si="8"/>
+        <v>229.41176470588235</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
+      </c>
       <c r="X21" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y21" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1999,17 +3130,36 @@
         <v>69</v>
       </c>
       <c r="R22">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S22">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="T22">
+        <v>41</v>
+      </c>
+      <c r="U22" s="3">
+        <f t="shared" si="8"/>
+        <v>241.1764705882353</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W22" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X22" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y22" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2070,17 +3220,36 @@
         <v>70</v>
       </c>
       <c r="R23">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S23">
-        <v>147</v>
+        <v>156</v>
+      </c>
+      <c r="T23">
+        <v>43</v>
+      </c>
+      <c r="U23" s="3">
+        <f t="shared" si="8"/>
+        <v>275.64102564102564</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W23" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X23" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y23" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2141,17 +3310,36 @@
         <v>73</v>
       </c>
       <c r="R24">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S24">
-        <v>161</v>
+        <v>169</v>
+      </c>
+      <c r="T24">
+        <v>45</v>
+      </c>
+      <c r="U24" s="3">
+        <f t="shared" si="8"/>
+        <v>266.27218934911247</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X24" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y24" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2212,17 +3400,36 @@
         <v>72</v>
       </c>
       <c r="R25">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S25">
-        <v>192</v>
+        <v>177</v>
+      </c>
+      <c r="T25">
+        <v>47</v>
+      </c>
+      <c r="U25" s="3">
+        <f t="shared" si="8"/>
+        <v>265.53672316384183</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X25" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y25" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2283,17 +3490,36 @@
         <v>80</v>
       </c>
       <c r="R26">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S26">
-        <v>165</v>
+        <v>172</v>
+      </c>
+      <c r="T26">
+        <v>49</v>
+      </c>
+      <c r="U26" s="3">
+        <f t="shared" si="8"/>
+        <v>284.88372093023258</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X26" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y26" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2354,17 +3580,36 @@
         <v>79</v>
       </c>
       <c r="R27">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S27">
-        <v>158</v>
+        <v>167</v>
+      </c>
+      <c r="T27">
+        <v>51</v>
+      </c>
+      <c r="U27" s="3">
+        <f t="shared" si="8"/>
+        <v>305.38922155688624</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X27" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y27" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2425,17 +3670,36 @@
         <v>81</v>
       </c>
       <c r="R28">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S28">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="T28">
+        <v>53</v>
+      </c>
+      <c r="U28" s="3">
+        <f t="shared" si="8"/>
+        <v>319.2771084337349</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X28" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y28" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2496,17 +3760,36 @@
         <v>88</v>
       </c>
       <c r="R29">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S29">
-        <v>170</v>
+        <v>167</v>
+      </c>
+      <c r="T29">
+        <v>55</v>
+      </c>
+      <c r="U29" s="3">
+        <f t="shared" si="8"/>
+        <v>329.34131736526945</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X29" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y29" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2567,17 +3850,36 @@
         <v>89</v>
       </c>
       <c r="R30">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S30">
-        <v>171</v>
+        <v>187</v>
+      </c>
+      <c r="T30">
+        <v>57</v>
+      </c>
+      <c r="U30" s="3">
+        <f t="shared" si="8"/>
+        <v>304.81283422459893</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X30" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y30" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2638,17 +3940,36 @@
         <v>89</v>
       </c>
       <c r="R31">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S31">
-        <v>176</v>
+        <v>159</v>
+      </c>
+      <c r="T31">
+        <v>59</v>
+      </c>
+      <c r="U31" s="3">
+        <f t="shared" si="8"/>
+        <v>371.06918238993705</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X31" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y31" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2709,17 +4030,36 @@
         <v>98</v>
       </c>
       <c r="R32">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S32">
-        <v>144</v>
+        <v>178</v>
+      </c>
+      <c r="T32">
+        <v>61</v>
+      </c>
+      <c r="U32" s="3">
+        <f t="shared" si="8"/>
+        <v>342.69662921348316</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W32" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X32" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y32" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2780,17 +4120,36 @@
         <v>97</v>
       </c>
       <c r="R33">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S33">
-        <v>170</v>
+        <v>161</v>
+      </c>
+      <c r="T33">
+        <v>63</v>
+      </c>
+      <c r="U33" s="3">
+        <f t="shared" si="8"/>
+        <v>391.304347826087</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W33" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X33" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y33" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2851,12 +4210,31 @@
         <v>99</v>
       </c>
       <c r="R34">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S34">
-        <v>173</v>
+        <v>159</v>
+      </c>
+      <c r="T34">
+        <v>65</v>
+      </c>
+      <c r="U34" s="3">
+        <f t="shared" si="8"/>
+        <v>408.80503144654091</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="9"/>
+        <v>Comb</v>
+      </c>
+      <c r="W34" t="str">
+        <f t="shared" si="10"/>
+        <v>Seq</v>
       </c>
       <c r="X34" t="str">
+        <f t="shared" si="11"/>
+        <v>Seq</v>
+      </c>
+      <c r="Y34" t="str">
         <f t="shared" si="7"/>
         <v>Seq</v>
       </c>
@@ -2872,7 +4250,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2958,10 +4336,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>